<commit_message>
Expanded excel_feature to include function to add the dates to each day of the week and generate a dated output file and one, incorporated into the final shift generating functions of each department, to add the shifts to the worksheet.
</commit_message>
<xml_diff>
--- a/blank_week.xlsx
+++ b/blank_week.xlsx
@@ -568,7 +568,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
@@ -653,88 +653,63 @@
       <c r="I3" s="21" t="n"/>
     </row>
     <row r="4" ht="15.75" customHeight="1" s="13">
-      <c r="A4" s="18" t="inlineStr">
+      <c r="A4" s="12" t="inlineStr">
+        <is>
+          <t>Rune, Jackson</t>
+        </is>
+      </c>
+      <c r="B4" s="12" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" customHeight="1" s="13">
+      <c r="A5" s="12" t="inlineStr">
+        <is>
+          <t>Montgomery, Lisa</t>
+        </is>
+      </c>
+      <c r="B5" s="12" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" ht="15.75" customHeight="1" s="13">
+      <c r="A6" s="12" t="inlineStr">
+        <is>
+          <t>McPhelan, Jon</t>
+        </is>
+      </c>
+      <c r="B6" s="12" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" ht="15.75" customHeight="1" s="13">
+      <c r="A7" s="12" t="inlineStr">
+        <is>
+          <t>Gravely, Tina</t>
+        </is>
+      </c>
+      <c r="B7" s="12" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" ht="15.75" customHeight="1" s="13">
+      <c r="A8" s="12" t="inlineStr">
+        <is>
+          <t>Doone, Perry</t>
+        </is>
+      </c>
+      <c r="B8" s="12" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" ht="15.75" customHeight="1" s="13">
+      <c r="A9" s="18" t="inlineStr">
         <is>
           <t>Shopfloor</t>
         </is>
       </c>
-      <c r="B4" s="19" t="n"/>
-      <c r="C4" s="22" t="n"/>
-      <c r="D4" s="19" t="n"/>
-      <c r="E4" s="19" t="n"/>
-      <c r="F4" s="19" t="n"/>
-      <c r="G4" s="19" t="n"/>
-      <c r="H4" s="19" t="n"/>
-      <c r="I4" s="19" t="n"/>
-    </row>
-    <row r="5" ht="15.75" customHeight="1" s="13">
-      <c r="A5" s="23" t="inlineStr">
-        <is>
-          <t>Eve</t>
-        </is>
-      </c>
-      <c r="B5" s="24" t="n"/>
-      <c r="C5" s="19" t="n"/>
-      <c r="D5" s="19" t="n"/>
-      <c r="E5" s="19" t="n"/>
-      <c r="F5" s="19" t="n"/>
-      <c r="G5" s="19" t="n"/>
-      <c r="H5" s="19" t="n"/>
-      <c r="I5" s="19" t="n"/>
-    </row>
-    <row r="6" ht="15.75" customHeight="1" s="13">
-      <c r="A6" s="23" t="inlineStr">
-        <is>
-          <t>Tills</t>
-        </is>
-      </c>
-      <c r="B6" s="24" t="n"/>
-      <c r="C6" s="19" t="n"/>
-      <c r="D6" s="19" t="n"/>
-      <c r="E6" s="19" t="n"/>
-      <c r="F6" s="19" t="n"/>
-      <c r="G6" s="19" t="n"/>
-      <c r="H6" s="19" t="n"/>
-      <c r="I6" s="19" t="n"/>
-    </row>
-    <row r="7" ht="15.75" customHeight="1" s="13">
-      <c r="A7" s="23" t="inlineStr">
-        <is>
-          <t>Showroom</t>
-        </is>
-      </c>
-      <c r="B7" s="24" t="n"/>
-      <c r="C7" s="19" t="n"/>
-      <c r="D7" s="19" t="n"/>
-      <c r="E7" s="19" t="n"/>
-      <c r="F7" s="19" t="n"/>
-      <c r="G7" s="19" t="n"/>
-      <c r="H7" s="19" t="n"/>
-      <c r="I7" s="23" t="n"/>
-    </row>
-    <row r="8" ht="15.75" customHeight="1" s="13">
-      <c r="A8" s="23" t="inlineStr">
-        <is>
-          <t>Warehouse</t>
-        </is>
-      </c>
-      <c r="B8" s="24" t="n"/>
-      <c r="C8" s="19" t="n"/>
-      <c r="D8" s="19" t="n"/>
-      <c r="E8" s="19" t="n"/>
-      <c r="F8" s="19" t="n"/>
-      <c r="G8" s="19" t="n"/>
-      <c r="H8" s="19" t="n"/>
-      <c r="I8" s="19" t="n"/>
-    </row>
-    <row r="9" ht="15.75" customHeight="1" s="13">
-      <c r="A9" s="23" t="inlineStr">
-        <is>
-          <t>Weekend</t>
-        </is>
-      </c>
-      <c r="B9" s="24" t="n"/>
-      <c r="C9" s="19" t="n"/>
+      <c r="B9" s="19" t="n"/>
+      <c r="C9" s="22" t="n"/>
       <c r="D9" s="19" t="n"/>
       <c r="E9" s="19" t="n"/>
       <c r="F9" s="19" t="n"/>
@@ -742,33 +717,301 @@
       <c r="H9" s="19" t="n"/>
       <c r="I9" s="19" t="n"/>
     </row>
-    <row r="10" ht="15.75" customHeight="1" s="13"/>
-    <row r="11" ht="15.75" customHeight="1" s="13"/>
-    <row r="12" ht="15.75" customHeight="1" s="13"/>
-    <row r="13" ht="15.75" customHeight="1" s="13"/>
-    <row r="14" ht="15.75" customHeight="1" s="13"/>
-    <row r="15" ht="15.75" customHeight="1" s="13"/>
-    <row r="16" ht="15.75" customHeight="1" s="13"/>
-    <row r="17" ht="15.75" customHeight="1" s="13"/>
-    <row r="18" ht="15.75" customHeight="1" s="13"/>
-    <row r="19" ht="15.75" customHeight="1" s="13"/>
-    <row r="20" ht="15.75" customHeight="1" s="13"/>
-    <row r="21" ht="15.75" customHeight="1" s="13"/>
-    <row r="22" ht="15.75" customHeight="1" s="13"/>
-    <row r="23" ht="13.5" customHeight="1" s="13"/>
-    <row r="24" ht="13.5" customHeight="1" s="13"/>
-    <row r="25" ht="13.5" customHeight="1" s="13"/>
-    <row r="26" ht="13.5" customHeight="1" s="13"/>
-    <row r="27" ht="13.5" customHeight="1" s="13"/>
-    <row r="28" ht="13.5" customHeight="1" s="13"/>
-    <row r="29" ht="13.5" customHeight="1" s="13"/>
-    <row r="30" ht="13.5" customHeight="1" s="13"/>
-    <row r="31" ht="13.5" customHeight="1" s="13"/>
-    <row r="32" ht="13.5" customHeight="1" s="13"/>
-    <row r="33" ht="13.5" customHeight="1" s="13"/>
-    <row r="34" ht="13.5" customHeight="1" s="13"/>
-    <row r="35" ht="13.5" customHeight="1" s="13"/>
-    <row r="36" ht="13.5" customHeight="1" s="13"/>
+    <row r="10" ht="15.75" customHeight="1" s="13">
+      <c r="A10" s="12" t="inlineStr">
+        <is>
+          <t>Roberts, Alexandra</t>
+        </is>
+      </c>
+      <c r="B10" s="12" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" ht="15.75" customHeight="1" s="13">
+      <c r="A11" s="12" t="inlineStr">
+        <is>
+          <t>Moorehouse, Alan</t>
+        </is>
+      </c>
+      <c r="B11" s="12" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" ht="15.75" customHeight="1" s="13">
+      <c r="A12" s="12" t="inlineStr">
+        <is>
+          <t>Montgomery, Annie</t>
+        </is>
+      </c>
+      <c r="B12" s="12" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" ht="15.75" customHeight="1" s="13">
+      <c r="A13" s="12" t="inlineStr">
+        <is>
+          <t>Farmer, Elizabeth</t>
+        </is>
+      </c>
+      <c r="B13" s="12" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" ht="15.75" customHeight="1" s="13">
+      <c r="A14" s="12" t="inlineStr">
+        <is>
+          <t>Chalmers, Ritchie</t>
+        </is>
+      </c>
+      <c r="B14" s="12" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" ht="15.75" customHeight="1" s="13">
+      <c r="A15" s="12" t="inlineStr">
+        <is>
+          <t>Ball, Tommy</t>
+        </is>
+      </c>
+      <c r="B15" s="12" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" ht="15.75" customHeight="1" s="13">
+      <c r="A16" s="23" t="inlineStr">
+        <is>
+          <t>Eve</t>
+        </is>
+      </c>
+      <c r="B16" s="24" t="n"/>
+      <c r="C16" s="19" t="n"/>
+      <c r="D16" s="19" t="n"/>
+      <c r="E16" s="19" t="n"/>
+      <c r="F16" s="19" t="n"/>
+      <c r="G16" s="19" t="n"/>
+      <c r="H16" s="19" t="n"/>
+      <c r="I16" s="19" t="n"/>
+    </row>
+    <row r="17" ht="15.75" customHeight="1" s="13">
+      <c r="A17" s="12" t="inlineStr">
+        <is>
+          <t>Montgomery, Cara</t>
+        </is>
+      </c>
+      <c r="B17" s="12" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" ht="15.75" customHeight="1" s="13">
+      <c r="A18" s="12" t="inlineStr">
+        <is>
+          <t>McAleer, George</t>
+        </is>
+      </c>
+      <c r="B18" s="12" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" ht="15.75" customHeight="1" s="13">
+      <c r="A19" s="12" t="inlineStr">
+        <is>
+          <t>Cunningham, Devontay</t>
+        </is>
+      </c>
+      <c r="B19" s="12" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" ht="15.75" customHeight="1" s="13">
+      <c r="A20" s="12" t="inlineStr">
+        <is>
+          <t>Barnet, Annie</t>
+        </is>
+      </c>
+      <c r="B20" s="12" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" ht="15.75" customHeight="1" s="13">
+      <c r="A21" s="23" t="inlineStr">
+        <is>
+          <t>Tills</t>
+        </is>
+      </c>
+      <c r="B21" s="24" t="n"/>
+      <c r="C21" s="19" t="n"/>
+      <c r="D21" s="19" t="n"/>
+      <c r="E21" s="19" t="n"/>
+      <c r="F21" s="19" t="n"/>
+      <c r="G21" s="19" t="n"/>
+      <c r="H21" s="19" t="n"/>
+      <c r="I21" s="19" t="n"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1" s="13">
+      <c r="A22" s="12" t="inlineStr">
+        <is>
+          <t>McKinty, Saoirse</t>
+        </is>
+      </c>
+      <c r="B22" s="12" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" ht="13.5" customHeight="1" s="13">
+      <c r="A23" s="12" t="inlineStr">
+        <is>
+          <t>Moon, Jaqui</t>
+        </is>
+      </c>
+      <c r="B23" s="12" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" ht="13.5" customHeight="1" s="13">
+      <c r="A24" s="12" t="inlineStr">
+        <is>
+          <t>Juniper, Sia</t>
+        </is>
+      </c>
+      <c r="B24" s="12" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" ht="13.5" customHeight="1" s="13">
+      <c r="A25" s="23" t="inlineStr">
+        <is>
+          <t>Showroom</t>
+        </is>
+      </c>
+      <c r="B25" s="24" t="n"/>
+      <c r="C25" s="19" t="n"/>
+      <c r="D25" s="19" t="n"/>
+      <c r="E25" s="19" t="n"/>
+      <c r="F25" s="19" t="n"/>
+      <c r="G25" s="19" t="n"/>
+      <c r="H25" s="19" t="n"/>
+      <c r="I25" s="23" t="n"/>
+    </row>
+    <row r="26" ht="13.5" customHeight="1" s="13">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Snell, Gabby</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" ht="13.5" customHeight="1" s="13">
+      <c r="A27" s="12" t="inlineStr">
+        <is>
+          <t>McClintock, Greg</t>
+        </is>
+      </c>
+      <c r="B27" s="12" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" ht="13.5" customHeight="1" s="13">
+      <c r="A28" s="23" t="inlineStr">
+        <is>
+          <t>Warehouse</t>
+        </is>
+      </c>
+      <c r="B28" s="24" t="n"/>
+      <c r="C28" s="19" t="n"/>
+      <c r="D28" s="19" t="n"/>
+      <c r="E28" s="19" t="n"/>
+      <c r="F28" s="19" t="n"/>
+      <c r="G28" s="19" t="n"/>
+      <c r="H28" s="19" t="n"/>
+      <c r="I28" s="19" t="n"/>
+    </row>
+    <row r="29" ht="13.5" customHeight="1" s="13">
+      <c r="A29" s="12" t="inlineStr">
+        <is>
+          <t>O'Hanlon, Neil</t>
+        </is>
+      </c>
+      <c r="B29" s="12" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" ht="13.5" customHeight="1" s="13">
+      <c r="A30" s="12" t="inlineStr">
+        <is>
+          <t>McElrea, Sean</t>
+        </is>
+      </c>
+      <c r="B30" s="12" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" ht="13.5" customHeight="1" s="13">
+      <c r="A31" s="12" t="inlineStr">
+        <is>
+          <t>Fortuna, Mika</t>
+        </is>
+      </c>
+      <c r="B31" s="12" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" ht="13.5" customHeight="1" s="13">
+      <c r="A32" s="23" t="inlineStr">
+        <is>
+          <t>Weekend</t>
+        </is>
+      </c>
+      <c r="B32" s="24" t="n"/>
+      <c r="C32" s="19" t="n"/>
+      <c r="D32" s="19" t="n"/>
+      <c r="E32" s="19" t="n"/>
+      <c r="F32" s="19" t="n"/>
+      <c r="G32" s="19" t="n"/>
+      <c r="H32" s="19" t="n"/>
+      <c r="I32" s="19" t="n"/>
+    </row>
+    <row r="33" ht="13.5" customHeight="1" s="13">
+      <c r="A33" s="12" t="inlineStr">
+        <is>
+          <t>McKinty, Cara</t>
+        </is>
+      </c>
+      <c r="B33" s="12" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" ht="13.5" customHeight="1" s="13">
+      <c r="A34" s="12" t="inlineStr">
+        <is>
+          <t>Krabb, Casey</t>
+        </is>
+      </c>
+      <c r="B34" s="12" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" ht="13.5" customHeight="1" s="13">
+      <c r="A35" s="12" t="inlineStr">
+        <is>
+          <t>Carter, Ovince</t>
+        </is>
+      </c>
+      <c r="B35" s="12" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" ht="13.5" customHeight="1" s="13">
+      <c r="A36" s="12" t="inlineStr">
+        <is>
+          <t>Cooper, Simon</t>
+        </is>
+      </c>
+      <c r="B36" s="12" t="n">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="A1:A2"/>

</xml_diff>